<commit_message>
modified a lot as JMC demanded
</commit_message>
<xml_diff>
--- a/SH_OBD/Configs/OBD_Result.xlsx
+++ b/SH_OBD/Configs/OBD_Result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\SH_OBD\SH_OBD\bin\Debug\Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\SH_OBD\SH_OBD\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB2C9A6-0137-41D4-9445-732CDE12DD16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D844F9-482C-437A-A2F1-1021EBE87290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B031C48-3480-47E7-B6F7-2E04DE9B3595}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>（1）车辆信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,43 +68,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OBD故障指示器状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OBD故障指示器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>与OBD诊断仪通讯情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OBD故障指示器被点亮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>故障代码及故障信息（如有）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>诊断就绪状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>诊断就绪状态未完成项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIL灯点亮后行驶里程（km）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>检测结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验员：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduleID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -137,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -161,26 +137,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -230,65 +186,44 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -384,7 +319,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACE"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -673,135 +608,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC24CF6-F44C-472A-805F-B005B97B8B60}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="4" max="5" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
+      <c r="E9" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fixbug: auto upload with result = 0
</commit_message>
<xml_diff>
--- a/SH_OBD/Configs/OBD_Result.xlsx
+++ b/SH_OBD/Configs/OBD_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\SH_OBD\SH_OBD\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D844F9-482C-437A-A2F1-1021EBE87290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94AE04E-922F-46A9-8475-8D8D98A79481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B031C48-3480-47E7-B6F7-2E04DE9B3595}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>（1）车辆信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,10 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（2）OBD检查信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>与OBD诊断仪通讯情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -81,6 +77,18 @@
   </si>
   <si>
     <t>moduleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（3）OBD检查信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（2）外观检验信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外观检验结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -608,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC24CF6-F44C-472A-805F-B005B97B8B60}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -639,7 +647,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -677,7 +685,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -685,17 +693,17 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -703,13 +711,31 @@
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fixbug: read data from J1939 with multi-package
</commit_message>
<xml_diff>
--- a/SH_OBD/Configs/OBD_Result.xlsx
+++ b/SH_OBD/Configs/OBD_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\SH_OBD\SH_OBD\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59A276-5E71-4D29-966F-5003ADEF9932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BB8FD8-7367-4A71-9E5E-3465202F2E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B031C48-3480-47E7-B6F7-2E04DE9B3595}"/>
   </bookViews>
@@ -208,7 +208,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -241,6 +241,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -335,7 +341,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CEEACA"/>
+        <a:sysClr val="window" lastClr="CAEACE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -627,7 +633,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -704,7 +710,7 @@
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="7"/>
@@ -722,7 +728,7 @@
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="7"/>
@@ -731,7 +737,7 @@
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="7"/>
@@ -740,7 +746,7 @@
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="7"/>
@@ -749,7 +755,7 @@
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>

</xml_diff>

<commit_message>
adjust connection sequence of protocol
</commit_message>
<xml_diff>
--- a/SH_OBD/Configs/OBD_Result.xlsx
+++ b/SH_OBD/Configs/OBD_Result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\SH_OBD\SH_OBD\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BB8FD8-7367-4A71-9E5E-3465202F2E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB1004A-1B3F-4BFE-A9C3-BEC8A6DA1AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B031C48-3480-47E7-B6F7-2E04DE9B3595}"/>
   </bookViews>
@@ -633,7 +633,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -755,7 +755,7 @@
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>

</xml_diff>